<commit_message>
Skip generation of volsmile and q-probability if already exists
</commit_message>
<xml_diff>
--- a/data_processed/market_objects.xlsx
+++ b/data_processed/market_objects.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B87"/>
+  <dimension ref="A1:B95"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1461,7 +1461,7 @@
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>['USD.SOFR.CSA_USD', 'BTCUSD.SPOT']</t>
+          <t>['USD.SOFR.CSA_USD', 'BTCUSD.SPOT', 'BTC.FUNDING.CSA_USD', 'BTCUSD.VOLSURFACE']</t>
         </is>
       </c>
     </row>
@@ -1472,6 +1472,102 @@
         </is>
       </c>
       <c r="B87" t="inlineStr">
+        <is>
+          <t>['BTCUSD.SPOT']</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>2025-09-07</t>
+        </is>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>['BTCUSD.SPOT']</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>2025-09-08</t>
+        </is>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>['USD.SOFR.CSA_USD', 'BTCUSD.SPOT', 'BTC.FUNDING.CSA_USD', 'BTCUSD.VOLSURFACE']</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>2025-09-09</t>
+        </is>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>['USD.SOFR.CSA_USD', 'BTCUSD.SPOT', 'BTC.FUNDING.CSA_USD', 'BTCUSD.VOLSURFACE']</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>2025-09-10</t>
+        </is>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>['USD.SOFR.CSA_USD', 'BTCUSD.SPOT', 'BTC.FUNDING.CSA_USD', 'BTCUSD.VOLSURFACE']</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>2025-09-11</t>
+        </is>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>['USD.SOFR.CSA_USD', 'BTCUSD.SPOT', 'BTC.FUNDING.CSA_USD', 'BTCUSD.VOLSURFACE']</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>2025-09-12</t>
+        </is>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>['USD.SOFR.CSA_USD', 'BTCUSD.SPOT']</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>2025-09-13</t>
+        </is>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>2025-09-14</t>
+        </is>
+      </c>
+      <c r="B95" t="inlineStr">
         <is>
           <t>[]</t>
         </is>

</xml_diff>

<commit_message>
updated smoothed volsurface and q^probability
</commit_message>
<xml_diff>
--- a/data_processed/market_objects.xlsx
+++ b/data_processed/market_objects.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B95"/>
+  <dimension ref="A1:B100"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1545,7 +1545,7 @@
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>['USD.SOFR.CSA_USD', 'BTCUSD.SPOT']</t>
+          <t>['USD.SOFR.CSA_USD', 'BTCUSD.SPOT', 'BTC.FUNDING.CSA_USD', 'BTCUSD.VOLSURFACE']</t>
         </is>
       </c>
     </row>
@@ -1557,7 +1557,7 @@
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>['BTCUSD.SPOT']</t>
         </is>
       </c>
     </row>
@@ -1569,7 +1569,67 @@
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>['BTCUSD.SPOT']</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>2025-09-15</t>
+        </is>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>['USD.SOFR.CSA_USD', 'BTCUSD.SPOT', 'BTC.FUNDING.CSA_USD', 'BTCUSD.VOLSURFACE']</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>2025-09-16</t>
+        </is>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>['USD.SOFR.CSA_USD', 'BTCUSD.SPOT', 'BTC.FUNDING.CSA_USD', 'BTCUSD.VOLSURFACE']</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>2025-09-17</t>
+        </is>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>['USD.SOFR.CSA_USD', 'BTCUSD.SPOT', 'BTC.FUNDING.CSA_USD', 'BTCUSD.VOLSURFACE']</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="inlineStr">
+        <is>
+          <t>2025-09-18</t>
+        </is>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>['USD.SOFR.CSA_USD', 'BTCUSD.SPOT']</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="inlineStr">
+        <is>
+          <t>2025-09-19</t>
+        </is>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>['USD.SOFR.CSA_USD']</t>
         </is>
       </c>
     </row>

</xml_diff>